<commit_message>
Atualização via Dashboard Streamlit
</commit_message>
<xml_diff>
--- a/dados_obras_v5.xlsx
+++ b/dados_obras_v5.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,50 +471,40 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Mat_Orc</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Mat_Real</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Desp_Real</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>HH_Orc_Qtd</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>HH_Real_Qtd</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>HH_Real_Vlr</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Impostos</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Mat_Orc</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Mat_Real</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Desp_Orc</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Desp_Real</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>HH_Orc_Vlr</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>HH_Real_Vlr</t>
-        </is>
-      </c>
       <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>HH_Orc_Qtd</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>HH_Real_Qtd</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Conclusao_%</t>
         </is>
@@ -523,211 +513,193 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024.0824</t>
+          <t>PRJ-2026001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Climatização Casa de Força</t>
+          <t>Automação Linha 2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BP</t>
+          <t>Ambev</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Pedro Afonso</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Finalizado</t>
+          <t>Em andamento</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>882000</v>
+        <v>263256.66</v>
       </c>
       <c r="G2" t="n">
-        <v>1764000</v>
+        <v>129800.53</v>
       </c>
       <c r="H2" t="n">
-        <v>172254.6</v>
+        <v>78167.08</v>
       </c>
       <c r="I2" t="n">
-        <v>287248</v>
+        <v>106830.93</v>
       </c>
       <c r="J2" t="n">
-        <v>245067</v>
+        <v>21366.19</v>
       </c>
       <c r="K2" t="n">
-        <v>149758</v>
+        <v>644</v>
       </c>
       <c r="L2" t="n">
-        <v>178732</v>
+        <v>1068</v>
       </c>
       <c r="M2" t="n">
-        <v>87312</v>
+        <v>85464.75</v>
       </c>
       <c r="N2" t="n">
-        <v>16271</v>
+        <v>43437.35</v>
       </c>
       <c r="O2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="P2" t="n">
-        <v>350</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025.0452</t>
+          <t>PRJ-2026002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Infra Gás GLP Pesquisa</t>
+          <t>Manutenção Preventiva</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bayer</t>
+          <t>Gerdau</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Uberlândia</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Finalizado</t>
+          <t>Em andamento</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>20000</v>
+        <v>306361.43</v>
       </c>
       <c r="G3" t="n">
-        <v>20000</v>
+        <v>141305.28</v>
       </c>
       <c r="H3" t="n">
-        <v>3906</v>
+        <v>83077.17</v>
       </c>
       <c r="I3" t="n">
-        <v>3350</v>
+        <v>97269.75999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>2100</v>
+        <v>19453.95</v>
       </c>
       <c r="K3" t="n">
-        <v>2956</v>
+        <v>673</v>
       </c>
       <c r="L3" t="n">
-        <v>1467</v>
+        <v>972</v>
       </c>
       <c r="M3" t="n">
-        <v>4957</v>
+        <v>77815.8</v>
       </c>
       <c r="N3" t="n">
-        <v>457</v>
+        <v>50549.64</v>
       </c>
       <c r="O3" t="n">
-        <v>100</v>
-      </c>
-      <c r="P3" t="n">
-        <v>12</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>100</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025.0607</t>
+          <t>PRJ-2026003</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Elétrica Refeitório</t>
+          <t>Automação Linha 2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Engetrad</t>
+          <t>Petrobras</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Pedro Afonso</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Finalizado</t>
+          <t>Em andamento</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>66000</v>
+        <v>55371.73</v>
       </c>
       <c r="G4" t="n">
-        <v>66000</v>
+        <v>37898.65</v>
       </c>
       <c r="H4" t="n">
-        <v>12889.8</v>
+        <v>17436.76</v>
       </c>
       <c r="I4" t="n">
-        <v>11290</v>
+        <v>22004.4</v>
       </c>
       <c r="J4" t="n">
-        <v>5139</v>
+        <v>4400.88</v>
       </c>
       <c r="K4" t="n">
-        <v>13771</v>
+        <v>173</v>
       </c>
       <c r="L4" t="n">
-        <v>1356</v>
+        <v>220</v>
       </c>
       <c r="M4" t="n">
-        <v>14586</v>
+        <v>17603.52</v>
       </c>
       <c r="N4" t="n">
-        <v>2458</v>
+        <v>9136.34</v>
       </c>
       <c r="O4" t="n">
-        <v>280</v>
-      </c>
-      <c r="P4" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025.1102</t>
+          <t>PRJ-2026004</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Reforma Painéis Elétricos</t>
+          <t>Subestação 13.8kV</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bayer</t>
+          <t>Klabin</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Uberlândia</t>
+          <t>Porto Alegre - RS</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -736,61 +708,55 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>45000</v>
+        <v>37153.58</v>
       </c>
       <c r="G5" t="n">
-        <v>20000</v>
+        <v>21042.67</v>
       </c>
       <c r="H5" t="n">
-        <v>8775</v>
+        <v>12872.56</v>
       </c>
       <c r="I5" t="n">
-        <v>12000</v>
+        <v>11714.59</v>
       </c>
       <c r="J5" t="n">
-        <v>13500</v>
+        <v>2342.92</v>
       </c>
       <c r="K5" t="n">
-        <v>3000</v>
+        <v>124</v>
       </c>
       <c r="L5" t="n">
-        <v>2800</v>
+        <v>117</v>
       </c>
       <c r="M5" t="n">
-        <v>8000</v>
+        <v>9371.67</v>
       </c>
       <c r="N5" t="n">
-        <v>5500</v>
+        <v>6130.34</v>
       </c>
       <c r="O5" t="n">
-        <v>200</v>
-      </c>
-      <c r="P5" t="n">
-        <v>140</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025.0888</t>
+          <t>PRJ-2026005</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Iluminação LED Industrial</t>
+          <t>Grupo Gerador</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bayer</t>
+          <t>Klabin</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Rio Verde</t>
+          <t>Recife - PE</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -799,103 +765,1459 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>150000</v>
+        <v>7841119.68</v>
       </c>
       <c r="G6" t="n">
-        <v>50000</v>
+        <v>5377258.5</v>
       </c>
       <c r="H6" t="n">
-        <v>29250</v>
+        <v>1859502.7</v>
       </c>
       <c r="I6" t="n">
-        <v>70000</v>
+        <v>2489555.5</v>
       </c>
       <c r="J6" t="n">
-        <v>72000</v>
+        <v>497911.1</v>
       </c>
       <c r="K6" t="n">
-        <v>10000</v>
+        <v>19142</v>
       </c>
       <c r="L6" t="n">
-        <v>14000</v>
+        <v>24895</v>
       </c>
       <c r="M6" t="n">
-        <v>25000</v>
+        <v>1991644.4</v>
       </c>
       <c r="N6" t="n">
-        <v>28000</v>
+        <v>1293784.75</v>
       </c>
       <c r="O6" t="n">
-        <v>500</v>
-      </c>
-      <c r="P6" t="n">
-        <v>600</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025.2020</t>
+          <t>PRJ-2026006</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Subestação de Energia</t>
+          <t>Retrofit de Iluminação</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>JBS</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Apresentado</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>269147.72</v>
+      </c>
+      <c r="G7" t="n">
+        <v>183982.62</v>
+      </c>
+      <c r="H7" t="n">
+        <v>65987.23</v>
+      </c>
+      <c r="I7" t="n">
+        <v>85454.39999999999</v>
+      </c>
+      <c r="J7" t="n">
+        <v>17090.88</v>
+      </c>
+      <c r="K7" t="n">
+        <v>582</v>
+      </c>
+      <c r="L7" t="n">
+        <v>854</v>
+      </c>
+      <c r="M7" t="n">
+        <v>68363.52</v>
+      </c>
+      <c r="N7" t="n">
+        <v>44409.37</v>
+      </c>
+      <c r="O7" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PRJ-2026007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Adequação NR-10</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Braskem</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Curitiba - PR</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>14910616.3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5084507.45</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4219164.01</v>
+      </c>
+      <c r="I8" t="n">
+        <v>4083955.23</v>
+      </c>
+      <c r="J8" t="n">
+        <v>816791.05</v>
+      </c>
+      <c r="K8" t="n">
+        <v>47015</v>
+      </c>
+      <c r="L8" t="n">
+        <v>40839</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3267164.18</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2460251.69</v>
+      </c>
+      <c r="O8" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>PRJ-2026008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Retrofit de Iluminação</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Manaus - AM</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Apresentado</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>238522.5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>133808.81</v>
+      </c>
+      <c r="H9" t="n">
+        <v>81301.58</v>
+      </c>
+      <c r="I9" t="n">
+        <v>99646.14</v>
+      </c>
+      <c r="J9" t="n">
+        <v>19929.23</v>
+      </c>
+      <c r="K9" t="n">
+        <v>730</v>
+      </c>
+      <c r="L9" t="n">
+        <v>996</v>
+      </c>
+      <c r="M9" t="n">
+        <v>79716.91</v>
+      </c>
+      <c r="N9" t="n">
+        <v>39356.21</v>
+      </c>
+      <c r="O9" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>PRJ-2026009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Manutenção Preventiva</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Klabin</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Belo Horizonte - MG</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Finalizado</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>691600.22</v>
+      </c>
+      <c r="G10" t="n">
+        <v>668399.67</v>
+      </c>
+      <c r="H10" t="n">
+        <v>197831.6</v>
+      </c>
+      <c r="I10" t="n">
+        <v>183288.38</v>
+      </c>
+      <c r="J10" t="n">
+        <v>36657.68</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1843</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1832</v>
+      </c>
+      <c r="M10" t="n">
+        <v>146630.7</v>
+      </c>
+      <c r="N10" t="n">
+        <v>114114.04</v>
+      </c>
+      <c r="O10" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>PRJ-2026010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Instalação de SPDA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Gerdau</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Recife - PE</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Não iniciado</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>70689.92999999999</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>21871.48</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>236</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>17253.07</v>
+      </c>
+      <c r="N11" t="n">
+        <v>11663.84</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>PRJ-2026011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Instalação de SPDA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>JBS</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Salvador - BA</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Não iniciado</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>100930.76</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>29231.05</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>295</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>21870.56</v>
+      </c>
+      <c r="N12" t="n">
+        <v>16653.58</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PRJ-2026012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Subestação 13.8kV</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>Vale</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Canaã</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Salvador - BA</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>Em andamento</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>300000</v>
-      </c>
-      <c r="G7" t="n">
-        <v>100000</v>
-      </c>
-      <c r="H7" t="n">
-        <v>58500</v>
-      </c>
-      <c r="I7" t="n">
-        <v>140000</v>
-      </c>
-      <c r="J7" t="n">
-        <v>110000</v>
-      </c>
-      <c r="K7" t="n">
-        <v>20000</v>
-      </c>
-      <c r="L7" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M7" t="n">
-        <v>50000</v>
-      </c>
-      <c r="N7" t="n">
-        <v>30000</v>
-      </c>
-      <c r="O7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="P7" t="n">
-        <v>400</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>45</v>
+      <c r="F13" t="n">
+        <v>384775.01</v>
+      </c>
+      <c r="G13" t="n">
+        <v>282622.3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>148875.17</v>
+      </c>
+      <c r="I13" t="n">
+        <v>173903.81</v>
+      </c>
+      <c r="J13" t="n">
+        <v>34780.76</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1277</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1739</v>
+      </c>
+      <c r="M13" t="n">
+        <v>139123.05</v>
+      </c>
+      <c r="N13" t="n">
+        <v>63487.88</v>
+      </c>
+      <c r="O13" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>PRJ-2026013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Subestação 13.8kV</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Ambev</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Manaus - AM</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Não iniciado</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>7518695.36</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>2543449.8</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>23839</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1876135.01</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1240584.73</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>PRJ-2026014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Adequação NR-10</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Salvador - BA</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Apresentado</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>867283.67</v>
+      </c>
+      <c r="G15" t="n">
+        <v>483792.24</v>
+      </c>
+      <c r="H15" t="n">
+        <v>244585.1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>232056.48</v>
+      </c>
+      <c r="J15" t="n">
+        <v>46411.3</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2686</v>
+      </c>
+      <c r="L15" t="n">
+        <v>2320</v>
+      </c>
+      <c r="M15" t="n">
+        <v>185645.19</v>
+      </c>
+      <c r="N15" t="n">
+        <v>143101.81</v>
+      </c>
+      <c r="O15" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PRJ-2026015</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Montagem de Painéis</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Braskem</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Curitiba - PR</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Não iniciado</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>367315.26</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>101917.67</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1094</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>81314.75999999999</v>
+      </c>
+      <c r="N16" t="n">
+        <v>60607.02</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PRJ-2026016</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Cabeamento Estruturado</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Embraer</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>São Paulo - SP</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>467105.91</v>
+      </c>
+      <c r="G17" t="n">
+        <v>329268.79</v>
+      </c>
+      <c r="H17" t="n">
+        <v>165587.56</v>
+      </c>
+      <c r="I17" t="n">
+        <v>201127</v>
+      </c>
+      <c r="J17" t="n">
+        <v>40225.4</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1579</v>
+      </c>
+      <c r="L17" t="n">
+        <v>2011</v>
+      </c>
+      <c r="M17" t="n">
+        <v>160901.6</v>
+      </c>
+      <c r="N17" t="n">
+        <v>77072.47</v>
+      </c>
+      <c r="O17" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PRJ-2026017</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Subestação 13.8kV</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Braskem</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>São Paulo - SP</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>4714555.18</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2166043.32</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1423405.21</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1925297.3</v>
+      </c>
+      <c r="J18" t="n">
+        <v>385059.46</v>
+      </c>
+      <c r="K18" t="n">
+        <v>12710</v>
+      </c>
+      <c r="L18" t="n">
+        <v>19252</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1540237.84</v>
+      </c>
+      <c r="N18" t="n">
+        <v>777901.6</v>
+      </c>
+      <c r="O18" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PRJ-2026018</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Cabeamento Estruturado</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Klabin</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Curitiba - PR</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>875694.0600000001</v>
+      </c>
+      <c r="G19" t="n">
+        <v>402765.77</v>
+      </c>
+      <c r="H19" t="n">
+        <v>250776.38</v>
+      </c>
+      <c r="I19" t="n">
+        <v>237390.61</v>
+      </c>
+      <c r="J19" t="n">
+        <v>47478.12</v>
+      </c>
+      <c r="K19" t="n">
+        <v>2840</v>
+      </c>
+      <c r="L19" t="n">
+        <v>2373</v>
+      </c>
+      <c r="M19" t="n">
+        <v>189912.49</v>
+      </c>
+      <c r="N19" t="n">
+        <v>144489.52</v>
+      </c>
+      <c r="O19" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PRJ-2026019</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Cabeamento Estruturado</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Ambev</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Porto Alegre - RS</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Finalizado</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>134113.5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>127806.63</v>
+      </c>
+      <c r="H20" t="n">
+        <v>41065.12</v>
+      </c>
+      <c r="I20" t="n">
+        <v>55119.87</v>
+      </c>
+      <c r="J20" t="n">
+        <v>11023.97</v>
+      </c>
+      <c r="K20" t="n">
+        <v>340</v>
+      </c>
+      <c r="L20" t="n">
+        <v>551</v>
+      </c>
+      <c r="M20" t="n">
+        <v>44095.9</v>
+      </c>
+      <c r="N20" t="n">
+        <v>22128.73</v>
+      </c>
+      <c r="O20" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PRJ-2026020</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Instalação de SPDA</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Suzano</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Porto Alegre - RS</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Finalizado</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>127436.8</v>
+      </c>
+      <c r="G21" t="n">
+        <v>112614.17</v>
+      </c>
+      <c r="H21" t="n">
+        <v>31491.11</v>
+      </c>
+      <c r="I21" t="n">
+        <v>31335.49</v>
+      </c>
+      <c r="J21" t="n">
+        <v>6267.1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>360</v>
+      </c>
+      <c r="L21" t="n">
+        <v>313</v>
+      </c>
+      <c r="M21" t="n">
+        <v>25068.39</v>
+      </c>
+      <c r="N21" t="n">
+        <v>21027.07</v>
+      </c>
+      <c r="O21" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>PRJ-2026021</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Laudo Termográfico</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Recife - PE</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Apresentado</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>77112.50999999999</v>
+      </c>
+      <c r="G22" t="n">
+        <v>29046.84</v>
+      </c>
+      <c r="H22" t="n">
+        <v>23992.32</v>
+      </c>
+      <c r="I22" t="n">
+        <v>22724.66</v>
+      </c>
+      <c r="J22" t="n">
+        <v>4544.93</v>
+      </c>
+      <c r="K22" t="n">
+        <v>247</v>
+      </c>
+      <c r="L22" t="n">
+        <v>227</v>
+      </c>
+      <c r="M22" t="n">
+        <v>18179.73</v>
+      </c>
+      <c r="N22" t="n">
+        <v>12723.56</v>
+      </c>
+      <c r="O22" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PRJ-2026022</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Grupo Gerador</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Embraer</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Curitiba - PR</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Apresentado</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>794227.62</v>
+      </c>
+      <c r="G23" t="n">
+        <v>397586.5</v>
+      </c>
+      <c r="H23" t="n">
+        <v>263945.1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>246486.08</v>
+      </c>
+      <c r="J23" t="n">
+        <v>49297.22</v>
+      </c>
+      <c r="K23" t="n">
+        <v>2506</v>
+      </c>
+      <c r="L23" t="n">
+        <v>2464</v>
+      </c>
+      <c r="M23" t="n">
+        <v>197188.86</v>
+      </c>
+      <c r="N23" t="n">
+        <v>131047.56</v>
+      </c>
+      <c r="O23" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PRJ-2026023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Instalação de SPDA</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Recife - PE</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>11891468.94</v>
+      </c>
+      <c r="G24" t="n">
+        <v>9484792.630000001</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2675098.09</v>
+      </c>
+      <c r="I24" t="n">
+        <v>3775541.39</v>
+      </c>
+      <c r="J24" t="n">
+        <v>755108.28</v>
+      </c>
+      <c r="K24" t="n">
+        <v>30187</v>
+      </c>
+      <c r="L24" t="n">
+        <v>37755</v>
+      </c>
+      <c r="M24" t="n">
+        <v>3020433.11</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1962092.37</v>
+      </c>
+      <c r="O24" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PRJ-2026024</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Montagem de Painéis</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Braskem</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Salvador - BA</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Finalizado</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>366585.76</v>
+      </c>
+      <c r="G25" t="n">
+        <v>310172.83</v>
+      </c>
+      <c r="H25" t="n">
+        <v>113959.86</v>
+      </c>
+      <c r="I25" t="n">
+        <v>108215.22</v>
+      </c>
+      <c r="J25" t="n">
+        <v>21643.04</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1102</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1082</v>
+      </c>
+      <c r="M25" t="n">
+        <v>86572.17</v>
+      </c>
+      <c r="N25" t="n">
+        <v>60486.65</v>
+      </c>
+      <c r="O25" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>PRJ-2026025</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Projeto Elétrico</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Weg</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Finalizado</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>605692.37</v>
+      </c>
+      <c r="G26" t="n">
+        <v>574974.01</v>
+      </c>
+      <c r="H26" t="n">
+        <v>157175.12</v>
+      </c>
+      <c r="I26" t="n">
+        <v>153897.1</v>
+      </c>
+      <c r="J26" t="n">
+        <v>30779.42</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1762</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1538</v>
+      </c>
+      <c r="M26" t="n">
+        <v>123117.68</v>
+      </c>
+      <c r="N26" t="n">
+        <v>99939.24000000001</v>
+      </c>
+      <c r="O26" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>PRJ-2026026</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Laudo Termográfico</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Petrobras</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Manaus - AM</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Apresentado</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>2547659.3</v>
+      </c>
+      <c r="G27" t="n">
+        <v>292589.11</v>
+      </c>
+      <c r="H27" t="n">
+        <v>649561.9</v>
+      </c>
+      <c r="I27" t="n">
+        <v>808881.83</v>
+      </c>
+      <c r="J27" t="n">
+        <v>161776.37</v>
+      </c>
+      <c r="K27" t="n">
+        <v>5988</v>
+      </c>
+      <c r="L27" t="n">
+        <v>8088</v>
+      </c>
+      <c r="M27" t="n">
+        <v>647105.46</v>
+      </c>
+      <c r="N27" t="n">
+        <v>420363.78</v>
+      </c>
+      <c r="O27" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>PRJ-2026027</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Laudo Termográfico</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Ambev</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Porto Alegre - RS</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>631825.4399999999</v>
+      </c>
+      <c r="G28" t="n">
+        <v>208774.58</v>
+      </c>
+      <c r="H28" t="n">
+        <v>178420.57</v>
+      </c>
+      <c r="I28" t="n">
+        <v>175585.1</v>
+      </c>
+      <c r="J28" t="n">
+        <v>35117.02</v>
+      </c>
+      <c r="K28" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1755</v>
+      </c>
+      <c r="M28" t="n">
+        <v>140468.08</v>
+      </c>
+      <c r="N28" t="n">
+        <v>104251.2</v>
+      </c>
+      <c r="O28" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>PRJ-2026028</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Laudo Termográfico</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Braskem</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Salvador - BA</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Não iniciado</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>52283.09</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>14361.39</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>159</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>11056.29</v>
+      </c>
+      <c r="N29" t="n">
+        <v>8626.709999999999</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>PRJ-2026029</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Instalação de SPDA</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Weg</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Salvador - BA</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>871815.62</v>
+      </c>
+      <c r="G30" t="n">
+        <v>525856.25</v>
+      </c>
+      <c r="H30" t="n">
+        <v>217068.55</v>
+      </c>
+      <c r="I30" t="n">
+        <v>215364.94</v>
+      </c>
+      <c r="J30" t="n">
+        <v>43072.99</v>
+      </c>
+      <c r="K30" t="n">
+        <v>2335</v>
+      </c>
+      <c r="L30" t="n">
+        <v>2153</v>
+      </c>
+      <c r="M30" t="n">
+        <v>172291.95</v>
+      </c>
+      <c r="N30" t="n">
+        <v>143849.58</v>
+      </c>
+      <c r="O30" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>PRJ-2026030</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Automação Linha 2</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Weg</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Manaus - AM</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>2049551.42</v>
+      </c>
+      <c r="G31" t="n">
+        <v>844455.34</v>
+      </c>
+      <c r="H31" t="n">
+        <v>473852.28</v>
+      </c>
+      <c r="I31" t="n">
+        <v>650732.5699999999</v>
+      </c>
+      <c r="J31" t="n">
+        <v>130146.51</v>
+      </c>
+      <c r="K31" t="n">
+        <v>4646</v>
+      </c>
+      <c r="L31" t="n">
+        <v>6507</v>
+      </c>
+      <c r="M31" t="n">
+        <v>520586.06</v>
+      </c>
+      <c r="N31" t="n">
+        <v>338175.98</v>
+      </c>
+      <c r="O31" t="n">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>